<commit_message>
updates to the pintle test post mortem
</commit_message>
<xml_diff>
--- a/analysis/Pintle_V1 testing/Pintle Test 01-26-2019/00 Pintle Data Analysis 01-26-2019.xlsx
+++ b/analysis/Pintle_V1 testing/Pintle Test 01-26-2019/00 Pintle Data Analysis 01-26-2019.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE3ABA6-4D43-4C96-BBC6-875EE62F329C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B4A854-F22A-414F-881C-76DC356E1659}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9285" windowHeight="5640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Summary" sheetId="4" r:id="rId1"/>
@@ -599,37 +599,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -646,122 +616,17 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Experimental data</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Calculations!$G$13:$G$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.6219999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.1219999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.772000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.606999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.855999999999995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.986999999999995</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25.956999999999994</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>33.618000000000009</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28.463000000000008</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Calculations!$D$13:$D$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.7465000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.9926000000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.5804999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.8441000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.6189999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.0517000000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.69</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.878</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AEE1-4DAC-B452-A2C30CEDC6CC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Theoretical</c:v>
+            <c:v>Flow curve using average Cv</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -846,6 +711,117 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-AEE1-4DAC-B452-A2C30CEDC6CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Experimental data</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Calculations!$G$13:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.6219999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1219999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.772000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.606999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.855999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.986999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.956999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.618000000000009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.463000000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Calculations!$D$13:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.7465000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9926000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5804999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8441000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6189999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0517000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.878</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AEE1-4DAC-B452-A2C30CEDC6CC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1118,15 +1094,17 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.71629571303587058"/>
-          <c:y val="0.69108672736662635"/>
+          <c:x val="0.65466241219077204"/>
+          <c:y val="0.68574271903386841"/>
           <c:w val="0.27666026553817363"/>
           <c:h val="0.12129464948956854"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -7696,16 +7674,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7733,15 +7711,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>495301</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8543,8 +8521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:S117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B65" workbookViewId="0">
-      <selection activeCell="M82" sqref="M82"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>